<commit_message>
done some more clean up and commenting
</commit_message>
<xml_diff>
--- a/Inputdata Template (DO NOT CHANGE).xlsx
+++ b/Inputdata Template (DO NOT CHANGE).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4264522ea65d2ce8/Dokumenter/NTNU/Master/Python Code/Git Repo/Simple-System-for-Power-System-Reliability-Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1000" documentId="11_AD4D1D646341095ACB70008C251E688C5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED27E26B-C1DC-45D9-8119-B825E01718A6}"/>
+  <xr:revisionPtr revIDLastSave="1031" documentId="11_AD4D1D646341095ACB70008C251E688C5BDEDD88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F76B4EE-070A-46B5-8977-56B89DC65620}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="802" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Data" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Generation Data" sheetId="5" r:id="rId4"/>
     <sheet name="Backup Feeders" sheetId="6" r:id="rId5"/>
     <sheet name="Component Data" sheetId="4" r:id="rId6"/>
+    <sheet name="Weekly Load Factor" sheetId="7" r:id="rId7"/>
+    <sheet name="Daily Load Factor" sheetId="8" r:id="rId8"/>
+    <sheet name="Hourly Load Factor" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -265,30 +268,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{7E32AC18-1154-4C64-A7DF-420E36CCE58B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sondre Modalsli Aaberg:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Number of protection elements at section</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A2" authorId="0" shapeId="0" xr:uid="{726C4B52-C9F1-473E-A9EF-2B2ED8F01D6E}">
       <text>
         <r>
@@ -371,6 +350,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{92766C3C-A7BE-4424-A024-3C24774E2059}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sondre Modalsli Aaberg:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Peak load in MW, used for DERS and load curve</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{383D7EBB-2964-4F49-9485-85EC6ECB0F08}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sondre Modalsli Aaberg:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Number of customers, used for system indices</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A2" authorId="0" shapeId="0" xr:uid="{C4DD1FE2-F4DC-48F3-A171-873885B01EFD}">
       <text>
         <r>
@@ -405,6 +432,54 @@
     <author>Sondre Modalsli Aaberg</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E13A4148-E130-4A89-8F7D-F1B12C1B6258}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sondre Modalsli Aaberg:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Power capacity/generation of generation element (0 = infinite) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{B1E0791D-98F7-44A5-A09B-731900ADEC0F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sondre Modalsli Aaberg:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Energy capacity of storage BESS, set = 0 for generation and main feeder</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{C0B83DB0-A300-417D-B12E-A94A487637C8}">
       <text>
         <r>
@@ -451,6 +526,30 @@
           </rPr>
           <t xml:space="preserve">
 List of generation, same names as in buses sheet</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{8A4FBB3F-D2EF-402C-B44E-AE278234F552}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sondre Modalsli Aaberg:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Example of DERS</t>
         </r>
       </text>
     </comment>
@@ -488,6 +587,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2C34BADD-585F-4675-9046-2070A25C93B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sondre Modalsli Aaberg:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ends of the backup feeder</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{475F091A-8BB0-47FB-A32C-27EAC18DF007}">
       <text>
         <r>
@@ -623,7 +746,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>LP1</t>
   </si>
@@ -718,12 +841,6 @@
     <t>Lim MW</t>
   </si>
   <si>
-    <t>Lim MVAR</t>
-  </si>
-  <si>
-    <t>inf</t>
-  </si>
-  <si>
     <t>Main Feeder</t>
   </si>
   <si>
@@ -742,24 +859,15 @@
     <t>Nr Transformers</t>
   </si>
   <si>
-    <t>Nr Protection</t>
-  </si>
-  <si>
     <t>Fuse/breaker direction</t>
   </si>
   <si>
     <t>Disconnector direction</t>
   </si>
   <si>
-    <t>Breaker Type</t>
-  </si>
-  <si>
     <t>Transformer Type</t>
   </si>
   <si>
-    <t>Nr Breaker</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
@@ -770,6 +878,42 @@
   </si>
   <si>
     <t>BS1</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Load Factor</t>
+  </si>
+  <si>
+    <t>Day of week</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Winter Wkdy</t>
+  </si>
+  <si>
+    <t>Winter Wknd</t>
+  </si>
+  <si>
+    <t>Summer Wkdy</t>
+  </si>
+  <si>
+    <t>Summer Wknd</t>
+  </si>
+  <si>
+    <t>Spring/Fall Wkdy</t>
+  </si>
+  <si>
+    <t>Spring/Fall Wknd</t>
+  </si>
+  <si>
+    <t>E cap</t>
   </si>
 </sst>
 </file>
@@ -841,10 +985,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1176,15 +1316,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4E8D12-5BBA-4420-83A4-3BE8673EEFAA}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -1195,31 +1335,22 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1239,7 +1370,7 @@
         <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1247,14 +1378,8 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1274,7 +1399,7 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1282,14 +1407,8 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1309,7 +1428,7 @@
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1317,14 +1436,8 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1344,7 +1457,7 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1352,14 +1465,8 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1379,7 +1486,7 @@
         <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1387,14 +1494,8 @@
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1414,7 +1515,7 @@
         <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1422,14 +1523,8 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1449,7 +1544,7 @@
         <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1457,14 +1552,8 @@
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1484,18 +1573,12 @@
         <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
         <v>0</v>
       </c>
     </row>
@@ -1512,7 +1595,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF1C9F0-4343-4AD1-924D-ED1403BEA6CF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,24 +1709,38 @@
         <v>30</v>
       </c>
       <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1657,17 +1754,17 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>24</v>
@@ -1675,7 +1772,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -1698,7 +1795,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1808,7 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>24</v>
@@ -1719,7 +1816,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -1733,7 +1830,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>0.2</v>
@@ -1749,4 +1846,1112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970CE303-313E-4C62-8E87-DB16D535451C}">
+  <dimension ref="A1:B53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>83.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>84.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>83.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>73.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>72.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>72.099999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>75.400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>83.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>85.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>81.099999999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>88.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>89.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>80.099999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>77.599999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>72.599999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>74.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>74.400000000000006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>90.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>94.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>95.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF209977-B9AA-48FC-800B-7E7F77A86DBE}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF34848-B377-4627-B3E8-BBFD61608C42}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>67</v>
+      </c>
+      <c r="C2">
+        <v>78</v>
+      </c>
+      <c r="D2">
+        <v>64</v>
+      </c>
+      <c r="E2">
+        <v>74</v>
+      </c>
+      <c r="F2">
+        <v>63</v>
+      </c>
+      <c r="G2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>70</v>
+      </c>
+      <c r="F3">
+        <v>62</v>
+      </c>
+      <c r="G3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>68</v>
+      </c>
+      <c r="D4">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>66</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>59</v>
+      </c>
+      <c r="C5">
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <v>56</v>
+      </c>
+      <c r="E5">
+        <v>65</v>
+      </c>
+      <c r="F5">
+        <v>58</v>
+      </c>
+      <c r="G5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>59</v>
+      </c>
+      <c r="C6">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>56</v>
+      </c>
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6">
+        <v>59</v>
+      </c>
+      <c r="G6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>58</v>
+      </c>
+      <c r="E7">
+        <v>62</v>
+      </c>
+      <c r="F7">
+        <v>65</v>
+      </c>
+      <c r="G7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>66</v>
+      </c>
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>62</v>
+      </c>
+      <c r="F8">
+        <v>72</v>
+      </c>
+      <c r="G8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>86</v>
+      </c>
+      <c r="C9">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>66</v>
+      </c>
+      <c r="F9">
+        <v>85</v>
+      </c>
+      <c r="G9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>95</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>87</v>
+      </c>
+      <c r="E10">
+        <v>81</v>
+      </c>
+      <c r="F10">
+        <v>95</v>
+      </c>
+      <c r="G10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>96</v>
+      </c>
+      <c r="C11">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <v>86</v>
+      </c>
+      <c r="F11">
+        <v>99</v>
+      </c>
+      <c r="G11">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>96</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>99</v>
+      </c>
+      <c r="E12">
+        <v>91</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>95</v>
+      </c>
+      <c r="C13">
+        <v>91</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <v>93</v>
+      </c>
+      <c r="F13">
+        <v>99</v>
+      </c>
+      <c r="G13">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>95</v>
+      </c>
+      <c r="C14">
+        <v>90</v>
+      </c>
+      <c r="D14">
+        <v>99</v>
+      </c>
+      <c r="E14">
+        <v>93</v>
+      </c>
+      <c r="F14">
+        <v>93</v>
+      </c>
+      <c r="G14">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>95</v>
+      </c>
+      <c r="C15">
+        <v>88</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>92</v>
+      </c>
+      <c r="F15">
+        <v>92</v>
+      </c>
+      <c r="G15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>93</v>
+      </c>
+      <c r="C16">
+        <v>87</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>91</v>
+      </c>
+      <c r="F16">
+        <v>90</v>
+      </c>
+      <c r="G16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>94</v>
+      </c>
+      <c r="C17">
+        <v>87</v>
+      </c>
+      <c r="D17">
+        <v>97</v>
+      </c>
+      <c r="E17">
+        <v>91</v>
+      </c>
+      <c r="F17">
+        <v>88</v>
+      </c>
+      <c r="G17">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>99</v>
+      </c>
+      <c r="C18">
+        <v>91</v>
+      </c>
+      <c r="D18">
+        <v>96</v>
+      </c>
+      <c r="E18">
+        <v>92</v>
+      </c>
+      <c r="F18">
+        <v>90</v>
+      </c>
+      <c r="G18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>96</v>
+      </c>
+      <c r="E19">
+        <v>94</v>
+      </c>
+      <c r="F19">
+        <v>92</v>
+      </c>
+      <c r="G19">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>99</v>
+      </c>
+      <c r="D20">
+        <v>93</v>
+      </c>
+      <c r="E20">
+        <v>95</v>
+      </c>
+      <c r="F20">
+        <v>96</v>
+      </c>
+      <c r="G20">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>96</v>
+      </c>
+      <c r="C21">
+        <v>97</v>
+      </c>
+      <c r="D21">
+        <v>92</v>
+      </c>
+      <c r="E21">
+        <v>95</v>
+      </c>
+      <c r="F21">
+        <v>98</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>91</v>
+      </c>
+      <c r="C22">
+        <v>94</v>
+      </c>
+      <c r="D22">
+        <v>92</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>96</v>
+      </c>
+      <c r="G22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>83</v>
+      </c>
+      <c r="C23">
+        <v>92</v>
+      </c>
+      <c r="D23">
+        <v>93</v>
+      </c>
+      <c r="E23">
+        <v>93</v>
+      </c>
+      <c r="F23">
+        <v>90</v>
+      </c>
+      <c r="G23">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>73</v>
+      </c>
+      <c r="C24">
+        <v>87</v>
+      </c>
+      <c r="D24">
+        <v>87</v>
+      </c>
+      <c r="E24">
+        <v>88</v>
+      </c>
+      <c r="F24">
+        <v>80</v>
+      </c>
+      <c r="G24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>63</v>
+      </c>
+      <c r="C25">
+        <v>81</v>
+      </c>
+      <c r="D25">
+        <v>72</v>
+      </c>
+      <c r="E25">
+        <v>80</v>
+      </c>
+      <c r="F25">
+        <v>70</v>
+      </c>
+      <c r="G25">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>